<commit_message>
[CHANGE] name in menu report
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_output_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_output_tax.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Output Tax Report" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sell Tax Report" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -350,7 +350,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>